<commit_message>
Removed blank rows to prevent "NA" when I import data
</commit_message>
<xml_diff>
--- a/eCAMI/taxa.xlsx
+++ b/eCAMI/taxa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\CRDS_Calcs\eCAMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B04A4C-CA10-49E5-BF32-986DCC9B1633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F939173D-FFB3-4B58-A818-8B5D3627F26C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36105" yWindow="2835" windowWidth="12195" windowHeight="8970" xr2:uid="{4801501B-AB0B-4627-9DF5-4F6E8F379054}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4801501B-AB0B-4627-9DF5-4F6E8F379054}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24304FE9-8396-4B28-B09D-5B10377A791E}">
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>